<commit_message>
Standardablauf steht, PlayPause-Buttons-Test in den Anfängen
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFDC4A7-B87B-430A-9FD2-36BF74A380E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,95 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
+  </si>
+  <si>
+    <t>Es wird im DropDown-Menü eine List aller möglichen Spieler angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt die Option "Mensch" im DropDown-Menü aus.</t>
+  </si>
+  <si>
+    <t>Als Spieler 1 wird ein Mensch festgelegt. Im DropDown-Menü wird angezeigt, dass die Option ausgewählt wurde.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 2.</t>
+  </si>
+  <si>
+    <t>Test: Standardablauf</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt die Option "KI 1" im DropDown-Menü aus.</t>
+  </si>
+  <si>
+    <t>Als Spieler 1 wird die "KI 1" festgelegt. Im DropDown-Menü wird angezeigt, dass die Option ausgewählt wurde.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Feld "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Der Graph zeigt das leere Feld und alle möglichen Folgezustände an.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf ein Feld des Spielfeldes.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird jetzt der Verlauf plus alle weiteren möglichen Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf den "Play-Pfeil".</t>
+  </si>
+  <si>
+    <t>Die KI macht einen zufälligen Zug und belegt somit ein zufälliges unbesetztes Feld. Dieses wird mit dem Zeichen "O" versehen. Im Graph wird der erneuerte Verlauf plus alle möglichen Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt abwechselnd auf ein freies Spielfeld und auf den "Play-Pfeil" bis das Spiel vorbei ist.</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den Verlauf plus alle weiteren möglichen Folgezustände an. Sobald das Spiel vorbei ist, wird das Spielergebnis angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf den Button "Neustart".</t>
+  </si>
+  <si>
+    <t>Die Spielerauswahl wird angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer behält die Konfiguration bei und klickt auf "Spiel starten"</t>
+  </si>
+  <si>
+    <t>Test: AutoPlay/Pause</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "Play"-Symbol</t>
+  </si>
+  <si>
+    <t>Das "Play"-Symbol wird durch ein "Pause"-Symbol ersetzt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "NextMove"-Symbol</t>
+  </si>
+  <si>
+    <t>Das "Pause"-Symbol wird durch ein "Play"-Symbol ersetzt. Es wird kein Zug ausgeführt, da der Mensch am Zug ist.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +422,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="94.21875" customWidth="1"/>
+    <col min="2" max="2" width="185.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoPlay/Pause, Doppelbesetzung und Spiel mit zwei Menschen steht
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFDC4A7-B87B-430A-9FD2-36BF74A380E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DE1073-77F8-455E-8F40-BCC403300F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird jetzt der Verlauf plus alle weiteren möglichen Folgezustände angezeigt.</t>
   </si>
   <si>
-    <t>Der Nutzer klickt auf den "Play-Pfeil".</t>
-  </si>
-  <si>
     <t>Die KI macht einen zufälligen Zug und belegt somit ein zufälliges unbesetztes Feld. Dieses wird mit dem Zeichen "O" versehen. Im Graph wird der erneuerte Verlauf plus alle möglichen Folgezustände angezeigt.</t>
   </si>
   <si>
@@ -87,16 +84,49 @@
     <t>Test: AutoPlay/Pause</t>
   </si>
   <si>
-    <t>Der Nutzer klickt auf das "Play"-Symbol</t>
-  </si>
-  <si>
-    <t>Das "Play"-Symbol wird durch ein "Pause"-Symbol ersetzt.</t>
-  </si>
-  <si>
-    <t>Der Nutzer klickt auf das "NextMove"-Symbol</t>
-  </si>
-  <si>
     <t>Das "Pause"-Symbol wird durch ein "Play"-Symbol ersetzt. Es wird kein Zug ausgeführt, da der Mensch am Zug ist.</t>
+  </si>
+  <si>
+    <t>Das "Play"-Symbol wird durch ein "Pause"-Symbol ersetzt. Es wird kein Zug ausgeführt, da der Mensch am Zug ist.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "NextMove"-Symbol.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf ein unbesetztes Feld des Spielfeldes.</t>
+  </si>
+  <si>
+    <t>Das "Play"-Symbol wird durch ein "Pause"-Symbol ersetzt. Die KI macht einen zufälligen Zug und belegt somit ein zufälliges unbesetztes Feld. Dieses wird mit dem Zeichen "O" versehen. Im Graph wird der erneuerte Verlauf plus alle möglichen Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird jetzt der Verlauf plus alle weiteren möglichen Folgezustände angezeigt. Kurze Zeit später macht die KI einen zufälligen Zug und belegt somit ein zufälliges unbesetztes Feld. Dieses wird mit dem Zeichen "O" versehen. Im Graph wird der erneuerte Verlauf plus alle möglichen Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Es passiert nichts, da das Feld bereits besetzt ist.</t>
+  </si>
+  <si>
+    <t>Test: Doppelbesetzung</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf ein bereits besetztes Feld des Spielfeldes.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "Pause"-Symbol.</t>
+  </si>
+  <si>
+    <t>Das "Pause"-Symbol wird durch ein "Play"-Symbol ersetzt.</t>
+  </si>
+  <si>
+    <t>Test: Spiel mit zwei Menschen</t>
+  </si>
+  <si>
+    <t>Als Spieler 2 wird ein Mensch festgelegt. Im DropDown-Menü wird angezeigt, dass die Option ausgewählt wurde.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "Play"-Symbol.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "O" versehen. Im Graph wird jetzt der Verlauf plus alle weiteren möglichen Folgezustände angezeigt.</t>
   </si>
 </sst>
 </file>
@@ -423,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,31 +520,31 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -522,23 +552,169 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardablauf ist jetzt gleich zum Epic aus dem ProductBacklog
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E97A0BA-4DC6-47F9-B480-2202CBE3C26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BCB310-21DB-4B9F-82EC-CE9BCA4CC7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 2.</t>
   </si>
   <si>
-    <t>Test: Standardablauf</t>
-  </si>
-  <si>
     <t>Der Nutzer wählt die Option "KI 1" im DropDown-Menü aus.</t>
   </si>
   <si>
@@ -66,21 +63,12 @@
     <t>Die KI macht einen zufälligen Zug und belegt somit ein zufälliges unbesetztes Feld. Dieses wird mit dem Zeichen "O" versehen. Im Graph wird der erneuerte Verlauf plus alle möglichen Folgezustände angezeigt.</t>
   </si>
   <si>
-    <t>Der Nutzer klickt abwechselnd auf ein freies Spielfeld und auf den "Play-Pfeil" bis das Spiel vorbei ist.</t>
-  </si>
-  <si>
-    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den Verlauf plus alle weiteren möglichen Folgezustände an. Sobald das Spiel vorbei ist, wird das Spielergebnis angezeigt.</t>
-  </si>
-  <si>
     <t>Der Nutzer klickt auf den Button "Neustart".</t>
   </si>
   <si>
     <t>Die Spielerauswahl wird angezeigt.</t>
   </si>
   <si>
-    <t>Der Nutzer behält die Konfiguration bei und klickt auf "Spiel starten"</t>
-  </si>
-  <si>
     <t>Test: AutoPlay/Pause</t>
   </si>
   <si>
@@ -130,6 +118,69 @@
   </si>
   <si>
     <t>Der Nutzer klickt auf "Spiel starten"</t>
+  </si>
+  <si>
+    <t>Es wird im DropDown-Menü eine Liste aller möglichen Spieler angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld oben links.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wechselt damit ab, auf ein zufälliges freies Spielfeld zu klicken und auf den Zug der KI zu warten, bis das Spiel vorbei ist.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf ein zufälliges freies Spielfeld.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Feld "Belohnung ausführen".</t>
+  </si>
+  <si>
+    <t>Es wird in den Startansicht gewechselt, in welchem die Spieler ausgewählt werden.</t>
+  </si>
+  <si>
+    <t>Test: Standardablauf/Epic</t>
+  </si>
+  <si>
+    <t>(Noch nicht implementiert: Die Checkbox wird mit einem Haken versehen.)</t>
+  </si>
+  <si>
+    <t>(Noch nicht implementiert: Der Nutzer klickt auf die Checkbox "Belohnungsansicht überspringen".)</t>
+  </si>
+  <si>
+    <t>(Noch nicht implementiert: Der Nutzer klickt auf die Checkbox "Startansicht überspringen".)</t>
+  </si>
+  <si>
+    <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Der Graph zeigt das leere Feld und alle Äquivalenzklassenvertreter der möglichen Folgezustände an.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Die KI macht einen zufälligen Zug und belegt somit ein zufälliges unbesetztes Feld. Dieses wird mit dem Zeichen "O" versehen. Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt. Ein zufälliges freies Feld wird von der KI besetzt und mit Zeichen "O" versehen.  Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. Sobald das Spiel vorbei ist, wird das Spielergebnis angezeigt. (Nicht implementiert: Es wird in die Belohnungsansicht gewechselt. Auf der rechten Seite wird als Graph der gesamte gewichtete Verlauf mit pro Zustand allen möglichen Äquivalenzklassenvertretern der Folgezuständen angezeigt.)</t>
+  </si>
+  <si>
+    <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Der Graph zeigt das leere Feld und alle möglichen Äquivalenzklassenvertreter der Folgezustände an.</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. (Noch nicht implementiert: Sobald das Spiel vorbei ist, wird direkt das Spielfeld geleert und der Verlauf-Graph auf das leere Feld mit allen möglichen Äquivalenzklassenvertretern der Folgezuständen geändert.)</t>
+  </si>
+  <si>
+    <t>(Noch nicht implementiert: Der Haken in der Checkbox wird entfernt.)</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. (Noch nicht implementiert: Sobald das Spiel vorbei ist, wird in die Startansicht gewechselt.)</t>
+  </si>
+  <si>
+    <t>(Noch nicht implementiert: Der Nutzer klickt auf das Feld "Reset KI" neben dem DropDown-Menü, in welchem die KI 1 ausgewählt ist.)</t>
+  </si>
+  <si>
+    <t>(Noch nicht implementiert: Es ändert sich nichts, da nur die Gewichte der KI gelöscht wurden.)</t>
   </si>
 </sst>
 </file>
@@ -456,21 +507,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="94.21875" customWidth="1"/>
-    <col min="2" max="2" width="185.77734375" customWidth="1"/>
+    <col min="1" max="1" width="124.109375" customWidth="1"/>
+    <col min="2" max="2" width="228.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -478,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -494,230 +545,294 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
+      <c r="B22" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
+      <c r="A31" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" t="s">
-        <v>33</v>
+      <c r="A35" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test AutoPlay/Pause ist jetzt selbstständig
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BCB310-21DB-4B9F-82EC-CE9BCA4CC7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5374D5EE-EFE3-4EF9-976C-20F5017454C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>(Noch nicht implementiert: Es ändert sich nichts, da nur die Gewichte der KI gelöscht wurden.)</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 "Mensch", für Spieler 2 "KI 1" und klickt auf das Feld "Spiel starten".</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,148 +678,148 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>18</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -824,7 +827,7 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -832,6 +835,14 @@
         <v>18</v>
       </c>
       <c r="B44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrationstest: Spielfeldbesetzung - Randfälle abgeschlossen
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A0333A-C1C7-4CDD-8626-DFD036BB308B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA5C427-7F64-4F09-90F1-347EB91EA71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -81,12 +81,6 @@
     <t>Es passiert nichts, da das Feld bereits besetzt ist.</t>
   </si>
   <si>
-    <t>Test: Doppelbesetzung</t>
-  </si>
-  <si>
-    <t>Der Nutzer klickt auf ein bereits besetztes Feld des Spielfeldes.</t>
-  </si>
-  <si>
     <t>Der Nutzer klickt auf das "Pause"-Symbol.</t>
   </si>
   <si>
@@ -202,6 +196,39 @@
   </si>
   <si>
     <t>Es wird in die Startansicht gewechselt, in welchem die Spieler ausgewählt werden.</t>
+  </si>
+  <si>
+    <t>Test: Spielfeldbesetzung - Randfälle</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld oben rechts.</t>
+  </si>
+  <si>
+    <t>Es passiert nichts, da der Spieler "Mensch" nicht an der Reihe ist.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das gerade von der KI ausgewählte Feld, welches mit einem "O" versehen wurde.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 "Mensch", für Spieler 2 "Mensch" und klickt auf das Feld "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld unten links.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "O" versehen. Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld oben in der Mitte.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld unten in der Mitte.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird der aktualisierte Verlauf ohne Äquivalenzklassenvertreter der Folgezustände angezeigt. Das Spielergebnis wird angezeigt: "Spieler 1 gewinnt!"</t>
+  </si>
+  <si>
+    <t>Es passiert nichts, da das Spiel bereits beendet ist.</t>
   </si>
 </sst>
 </file>
@@ -528,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,7 +569,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -550,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -566,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -582,28 +609,28 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -611,34 +638,34 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,47 +673,47 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -696,15 +723,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -720,18 +747,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -744,10 +771,10 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -755,23 +782,23 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -779,12 +806,12 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -792,58 +819,58 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -851,104 +878,216 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>21</v>
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>16</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Noch nicht implementiert:" rausgestrichen
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484ABC6B-66B6-45A4-B826-B21AD4680250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86011BCC-D779-4CF2-A732-B0F57B478A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,15 +120,6 @@
     <t>Test: Standardablauf/Epic</t>
   </si>
   <si>
-    <t>(Noch nicht implementiert: Die Checkbox wird mit einem Haken versehen.)</t>
-  </si>
-  <si>
-    <t>(Noch nicht implementiert: Der Nutzer klickt auf die Checkbox "Belohnungsansicht überspringen".)</t>
-  </si>
-  <si>
-    <t>(Noch nicht implementiert: Der Nutzer klickt auf die Checkbox "Startansicht überspringen".)</t>
-  </si>
-  <si>
     <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Der Graph zeigt das leere Feld und alle Äquivalenzklassenvertreter der möglichen Folgezustände an.</t>
   </si>
   <si>
@@ -141,27 +132,9 @@
     <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt. Ein zufälliges freies Feld wird von der KI besetzt und mit Zeichen "O" versehen.  Im Graph wird der aktualisierte Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände angezeigt.</t>
   </si>
   <si>
-    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. Sobald das Spiel vorbei ist, wird das Spielergebnis angezeigt. (Nicht implementiert: Es wird in die Belohnungsansicht gewechselt. Auf der rechten Seite wird als Graph der gesamte gewichtete Verlauf mit pro Zustand allen möglichen Äquivalenzklassenvertretern der Folgezuständen angezeigt.)</t>
-  </si>
-  <si>
-    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. (Noch nicht implementiert: Sobald das Spiel vorbei ist, wird direkt das Spielfeld geleert und der Verlauf-Graph auf das leere Feld mit allen möglichen Äquivalenzklassenvertretern der Folgezuständen geändert.)</t>
-  </si>
-  <si>
-    <t>(Noch nicht implementiert: Der Haken in der Checkbox wird entfernt.)</t>
-  </si>
-  <si>
-    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. (Noch nicht implementiert: Sobald das Spiel vorbei ist, wird in die Startansicht gewechselt.)</t>
-  </si>
-  <si>
-    <t>(Noch nicht implementiert: Es ändert sich nichts, da nur die Gewichte der KI gelöscht wurden.)</t>
-  </si>
-  <si>
     <t>Der Nutzer wählt für Spieler 1 "Mensch", für Spieler 2 "KI 1" und klickt auf das Feld "Spiel starten".</t>
   </si>
   <si>
-    <t>(Noch nicht implementiert: Der Nutzer klickt auf das Feld "Reset" neben KI 1.)</t>
-  </si>
-  <si>
     <t>Der Nutzer klickt auf dem Spielfeld auf das Feld unten rechts.</t>
   </si>
   <si>
@@ -244,6 +217,33 @@
   </si>
   <si>
     <t>Der Nutzer klickt auf dem Spielfeld auf das Feld in der Mitte rechts.</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. Sobald das Spiel vorbei ist, wird das Spielergebnis angezeigt. Es wird in die Belohnungsansicht gewechselt. Auf der rechten Seite wird als Graph der gesamte gewichtete Verlauf mit pro Zustand allen möglichen Äquivalenzklassenvertretern der Folgezuständen angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf die Checkbox "Startansicht überspringen".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Der Nutzer klickt auf die Checkbox "Belohnungsansicht überspringen".</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Feld "Reset" neben KI 1.</t>
+  </si>
+  <si>
+    <t>Es ändert sich nichts, da nur die Gewichte der KI gelöscht wurden.</t>
+  </si>
+  <si>
+    <t>Der Haken in der Checkbox wird entfernt.</t>
+  </si>
+  <si>
+    <t>Die Checkbox wird mit einem Haken versehen.</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. Sobald das Spiel vorbei ist, wird direkt das Spielfeld geleert und der Verlauf-Graph auf das leere Feld mit allen möglichen Äquivalenzklassenvertretern der Folgezuständen geändert.</t>
+  </si>
+  <si>
+    <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. Sobald das Spiel vorbei ist, wird in die Startansicht gewechselt.</t>
   </si>
 </sst>
 </file>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +624,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -632,15 +632,15 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -656,7 +656,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -664,7 +664,7 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,10 +677,10 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -688,15 +688,15 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -704,15 +704,15 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -720,15 +720,15 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -738,10 +738,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -762,10 +762,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -773,7 +773,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -786,10 +786,10 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -797,15 +797,15 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -821,7 +821,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -834,18 +834,18 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -853,15 +853,15 @@
         <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -877,7 +877,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -893,20 +893,20 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -914,15 +914,15 @@
         <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,12 +930,12 @@
         <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -951,10 +951,10 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -967,10 +967,10 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +978,7 @@
         <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -991,55 +991,55 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1047,71 +1047,71 @@
         <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Integrationstest: Spiel mit zwei Menschen abgeschlossen
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86011BCC-D779-4CF2-A732-B0F57B478A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FD43A0-E3F5-41DA-B8FE-6B65063327B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
   <si>
-    <t>Es wird im DropDown-Menü eine List aller möglichen Spieler angezeigt.</t>
-  </si>
-  <si>
     <t>Der Nutzer wählt die Option "Mensch" im DropDown-Menü aus.</t>
   </si>
   <si>
@@ -51,18 +48,6 @@
     <t>Der Nutzer klickt auf das Feld "Spiel starten".</t>
   </si>
   <si>
-    <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Der Graph zeigt das leere Feld und alle möglichen Folgezustände an.</t>
-  </si>
-  <si>
-    <t>Das angeklickte Feld wird mit dem Zeichen "X" versehen. Im Graph wird jetzt der Verlauf plus alle weiteren möglichen Folgezustände angezeigt.</t>
-  </si>
-  <si>
-    <t>Der Nutzer klickt auf den Button "Neustart".</t>
-  </si>
-  <si>
-    <t>Die Spielerauswahl wird angezeigt.</t>
-  </si>
-  <si>
     <t>Test: AutoPlay/Pause</t>
   </si>
   <si>
@@ -75,9 +60,6 @@
     <t>Der Nutzer klickt auf das "NextMove"-Symbol.</t>
   </si>
   <si>
-    <t>Der Nutzer klickt auf ein unbesetztes Feld des Spielfeldes.</t>
-  </si>
-  <si>
     <t>Es passiert nichts, da das Feld bereits besetzt ist.</t>
   </si>
   <si>
@@ -87,18 +69,9 @@
     <t>Test: Spiel mit zwei Menschen</t>
   </si>
   <si>
-    <t>Als Spieler 2 wird ein Mensch festgelegt. Im DropDown-Menü wird angezeigt, dass die Option ausgewählt wurde.</t>
-  </si>
-  <si>
     <t>Der Nutzer klickt auf das "Play"-Symbol.</t>
   </si>
   <si>
-    <t>Das angeklickte Feld wird mit dem Zeichen "O" versehen. Im Graph wird jetzt der Verlauf plus alle weiteren möglichen Folgezustände angezeigt.</t>
-  </si>
-  <si>
-    <t>Der Nutzer klickt auf "Spiel starten"</t>
-  </si>
-  <si>
     <t>Es wird im DropDown-Menü eine Liste aller möglichen Spieler angezeigt.</t>
   </si>
   <si>
@@ -244,6 +217,9 @@
   </si>
   <si>
     <t>Das Spielfeld wird laufend aktualisiert. Der Graph zeigt jeweils immer den aktualisierten Verlauf mit allen für die aktuelle Spielsituation möglichen Äquivalenzklassenvertretern der Folgezustände an. Sobald das Spiel vorbei ist, wird in die Startansicht gewechselt.</t>
+  </si>
+  <si>
+    <t>Führe Schritte von "Test: Spiel mit zwei Menschen" durch.</t>
   </si>
 </sst>
 </file>
@@ -570,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +560,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -592,603 +568,544 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>31</v>
+      <c r="A52" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>59</v>
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>52</v>
-      </c>
-      <c r="B62" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65" t="s">
-        <v>32</v>
+      <c r="A65" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B71" t="s">
-        <v>60</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>40</v>
+      </c>
+      <c r="B72" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>19</v>
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="B75" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B77" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>21</v>
-      </c>
-      <c r="B78" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>15</v>
-      </c>
-      <c r="B79" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>16</v>
-      </c>
-      <c r="B82" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrationstest haben jetzt Platz für Specs
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FD43A0-E3F5-41DA-B8FE-6B65063327B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD5BDA6-537F-486F-A6DB-C97431F52796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Gerätespecs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -548,22 +549,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="142.21875" customWidth="1"/>
-    <col min="2" max="2" width="228.109375" customWidth="1"/>
+    <col min="1" max="1" width="142.28515625" customWidth="1"/>
+    <col min="2" max="2" width="228.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -571,7 +572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -579,7 +580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -587,7 +588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -595,7 +596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -603,7 +604,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -611,7 +612,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -619,7 +620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -627,7 +628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -635,7 +636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -643,7 +644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -651,7 +652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -659,7 +660,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -667,7 +668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -675,7 +676,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -683,7 +684,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -691,7 +692,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -699,7 +700,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -707,12 +708,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -720,7 +721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -728,7 +729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -736,7 +737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -744,7 +745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -752,7 +753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -760,7 +761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -768,7 +769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -776,7 +777,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -784,7 +785,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -792,7 +793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -800,7 +801,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -808,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -816,7 +817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -824,7 +825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -832,7 +833,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -840,7 +841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -848,7 +849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -856,7 +857,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -864,7 +865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -872,12 +873,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -885,7 +886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -893,7 +894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -901,7 +902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -909,7 +910,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -917,7 +918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -925,7 +926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -933,12 +934,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -946,7 +947,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -954,7 +955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -962,7 +963,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -970,7 +971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -978,7 +979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -986,7 +987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -994,7 +995,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -1010,12 +1011,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -1023,12 +1024,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>52</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>46</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>53</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>54</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>44</v>
       </c>
@@ -1092,7 +1093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>27</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -1111,4 +1112,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651AFE88-806E-4574-AED0-363C8FFDCEFE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Zusätzlichen Integrationstest zum Slider geschrieben
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DA73A3-1E08-4097-B014-D1D929FD9ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA816A2-49F1-4B57-8FDA-6A5B58B7B629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="138">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -293,6 +293,153 @@
   </si>
   <si>
     <t>Die Gewichte der KI, die im Graphen angezeigt werden, ändern sich wie in der Definition der FehlerrückführungKI festgelegt.</t>
+  </si>
+  <si>
+    <t>Test: Spiel mit zwei KIs</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 "KI-Elimination", für Spieler 2 "KI-Fehlerrückführung" und klickt auf das Feld "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Der Graph ist im Ausgangszustand. Es stehen zwei Beschriftungen an den Kanten. Die Beschriftungen an den Kanten sind rot und blau gefärbt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "NextMove"-Symbol</t>
+  </si>
+  <si>
+    <t>Zufällige freie Felder werden von den KIs besetzt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "Play"-Symbol, bevor das Spiel beendet ist.</t>
+  </si>
+  <si>
+    <t>Keine weiteren Felder werden besetzt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Nutzer klickt auf das "Play"-Symbol und wartet bis das Spiel beendet ist. </t>
+  </si>
+  <si>
+    <t>Der Belohnungsbildschirm wird für die Evaluationsstrategie Elimination aufgerufen.</t>
+  </si>
+  <si>
+    <t>Der Belohnungsbildschirm wird für die Evaluationsstrategie Fehlerrückführung aufgerufen.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 2 "KI-Elimination".</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Es wird in die Spielansicht gewechselt. Das Feld ist leer und der Graph ist im Ausgangszustand.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "Play"-Symbol und wartet bis das Spiel beendet ist.</t>
+  </si>
+  <si>
+    <t>Der Spieler drückt auf "Weiter".</t>
+  </si>
+  <si>
+    <t>Test: KI erzeugen</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von "Wähle einen KI-Typ".</t>
+  </si>
+  <si>
+    <t>Es wird im DropDown-Menü eine Liste aller möglichen Spieler angezeigt. Die Optionen sind: "Elimination", "Fehlerrückführung", "Zufällig"</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt die Option "Elimination" im DropDown-Menü aus.</t>
+  </si>
+  <si>
+    <t>Im Feld des DropDown-Menüs für "Wähle einen KI-Typ" steht "Elimination".</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Feld "Wähle einen Namen für die KI".</t>
+  </si>
+  <si>
+    <t>Das Feld ist beschreibbar.</t>
+  </si>
+  <si>
+    <t>Der Nutzer schreibt "KI 1" in das Feld.</t>
+  </si>
+  <si>
+    <t>Im Feld "Wähle einen Namen für die KI" steht "KI 1".</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf "Erstelle eine neue KI".</t>
+  </si>
+  <si>
+    <t>In der Liste der KIs wird die neue KI angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt die Option "Fehlerrückführung" im DropDown-Menü aus.</t>
+  </si>
+  <si>
+    <t>Im Feld des DropDown-Menüs für "Wähle einen KI-Typ" steht "Fehlerrückführung".</t>
+  </si>
+  <si>
+    <t>Der Nutzer schreibt "KI 2" in das Feld.</t>
+  </si>
+  <si>
+    <t>Im Feld "Wähle einen Namen für die KI" steht "KI 2".</t>
+  </si>
+  <si>
+    <t>In der Liste wird die neue KI angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 "KI 1", für Spieler 2 "KI 2".</t>
+  </si>
+  <si>
+    <t>In den beiden Feldern steht "KI 1" und "KI 2".</t>
+  </si>
+  <si>
+    <t>Ein Spiel wird komplett durchgespielt und die KIs werden belohnt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt im Startbildschirm auf den Knopf "Zurücksetzen" neben der "KI 2".</t>
+  </si>
+  <si>
+    <t>Der Nutzer startet ein neues Spiel.</t>
+  </si>
+  <si>
+    <t>Die "KI 2" hat die gleichen Gewichte, wie beim ersten durchspielen.</t>
+  </si>
+  <si>
+    <t>Test: Slider</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 "KI-Elimination", für Spieler 2 "KI-Elimination" und klickt auf das Feld "Spiel starten".</t>
+  </si>
+  <si>
+    <t>In der Spielansicht existiert ein Slider, welcher auf ganz links eingestellt ist.</t>
+  </si>
+  <si>
+    <t>Der Nutzer bewegt den Slider nach ganz rechts.</t>
+  </si>
+  <si>
+    <t>Der Slider bewegt sich mit der Maus.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf den Slider, hält die Maus gedrückt und zieht sie nach ganz rechts und wieder nach ganz links.</t>
+  </si>
+  <si>
+    <t>Die Geschwindigkeit, mit der die KI die Züge macht erhöht sich.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wartet, bis das Spiel beendet ist, klickt auf "Weiter", "Belohnung ausführen", "Weiter" und auf "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Der Slider ist auf ganz rechts eingestellt und die KI macht ihre Züge weiterhin sehr schnell.</t>
+  </si>
+  <si>
+    <t>Test: Speedrun</t>
+  </si>
+  <si>
+    <t>Der Nutzer stellt den Slider auf ganz rechts.</t>
+  </si>
+  <si>
+    <t>Die KIs machen sehr schnell ihre Züge und es werden mehrere Spiele hintereinander ausgeführt.</t>
   </si>
 </sst>
 </file>
@@ -619,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,6 +1452,299 @@
       </c>
       <c r="B114" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>90</v>
+      </c>
+      <c r="B117" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>94</v>
+      </c>
+      <c r="B120" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>65</v>
+      </c>
+      <c r="B122" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>65</v>
+      </c>
+      <c r="B124" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>65</v>
+      </c>
+      <c r="B126" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>100</v>
+      </c>
+      <c r="B128" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>102</v>
+      </c>
+      <c r="B129" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>103</v>
+      </c>
+      <c r="B131" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>105</v>
+      </c>
+      <c r="B134" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>107</v>
+      </c>
+      <c r="B135" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>109</v>
+      </c>
+      <c r="B136" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>111</v>
+      </c>
+      <c r="B137" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>113</v>
+      </c>
+      <c r="B138" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>105</v>
+      </c>
+      <c r="B139" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>115</v>
+      </c>
+      <c r="B140" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>109</v>
+      </c>
+      <c r="B141" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>117</v>
+      </c>
+      <c r="B142" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>113</v>
+      </c>
+      <c r="B143" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>120</v>
+      </c>
+      <c r="B144" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>124</v>
+      </c>
+      <c r="B147" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>127</v>
+      </c>
+      <c r="B150" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B151" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>129</v>
+      </c>
+      <c r="B153" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>133</v>
+      </c>
+      <c r="B154" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>7</v>
+      </c>
+      <c r="B161" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kleine Änderungen an Integrationstests
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IAG-Leonid\Documents\Uni\ticTacToeTeamprojekt\Integrationstests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1F01BB-0949-4829-8C98-B8FC8A0790EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E95CB1-6BF7-4489-AFFA-7103EF60672A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>Der Graph ist im Ausgangszustand. Es stehen zwei Beschriftungen an den Kanten. Die Beschriftungen an den Kanten sind rot und blau gefärbt.</t>
   </si>
   <si>
-    <t>Der Nutzer klickt auf das "NextMove"-Symbol</t>
-  </si>
-  <si>
     <t>Zufällige freie Felder werden von den KIs besetzt.</t>
   </si>
   <si>
@@ -370,9 +367,6 @@
     <t>Der Nutzer klickt auf "Erstelle eine neue KI".</t>
   </si>
   <si>
-    <t>In der Liste der KIs wird die neue KI angezeigt.</t>
-  </si>
-  <si>
     <t>Der Nutzer wählt die Option "Fehlerrückführung" im DropDown-Menü aus.</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>Im Feld "Wähle einen Namen für die KI" steht "KI 2".</t>
   </si>
   <si>
-    <t>In der Liste wird die neue KI angezeigt.</t>
-  </si>
-  <si>
     <t>Der Nutzer wählt für Spieler 1 "KI 1", für Spieler 2 "KI 2".</t>
   </si>
   <si>
@@ -449,6 +440,15 @@
   </si>
   <si>
     <t>Die "KI 2" hat die gleichen Gewichte wie beim ersten durchspielen.</t>
+  </si>
+  <si>
+    <t>Im Startbildschirm ist auf der rechten Seite eine Liste mit allen existierenden KIs zu sehen. Die beiden Einträge sind initial "KI-Elimination" und "KI-Fehlerrückführung".</t>
+  </si>
+  <si>
+    <t>In der Liste der KIs wird die neue KI "KI 1" zusätzlich angezeigt.</t>
+  </si>
+  <si>
+    <t>In der Liste wird die neue KI zusätzlich angezeigt.</t>
   </si>
 </sst>
 </file>
@@ -778,21 +778,21 @@
   <dimension ref="A1:B161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.33203125" customWidth="1"/>
-    <col min="2" max="2" width="228.1328125" customWidth="1"/>
+    <col min="1" max="1" width="72.28515625" customWidth="1"/>
+    <col min="2" max="2" width="145.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -800,7 +800,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -808,7 +808,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -816,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -824,7 +824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -832,7 +832,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -840,7 +840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -848,7 +848,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -856,7 +856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -864,7 +864,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -872,7 +872,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -880,7 +880,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -888,7 +888,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -896,7 +896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -904,7 +904,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -912,7 +912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -920,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -928,7 +928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -936,7 +936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -944,7 +944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -952,17 +952,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -970,7 +970,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -978,7 +978,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -986,7 +986,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -994,7 +994,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1002,12 +1002,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1015,17 +1015,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1073,22 +1073,22 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1096,12 +1096,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -1109,15 +1109,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1125,15 +1125,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1149,17 +1149,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -1175,22 +1175,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1198,12 +1198,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -1219,17 +1219,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -1237,57 +1237,57 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>23</v>
       </c>
@@ -1295,27 +1295,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>74</v>
       </c>
@@ -1323,27 +1323,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>74</v>
       </c>
@@ -1351,27 +1351,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>74</v>
       </c>
@@ -1379,27 +1379,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>74</v>
       </c>
@@ -1407,27 +1407,27 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>74</v>
       </c>
@@ -1435,27 +1435,27 @@
         <v>88</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>74</v>
       </c>
@@ -1463,12 +1463,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>90</v>
       </c>
@@ -1476,284 +1476,285 @@
         <v>91</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="B119" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>94</v>
-      </c>
-      <c r="B120" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>65</v>
+      </c>
+      <c r="B121" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>65</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A123" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A124" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>65</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A126" t="s">
-        <v>65</v>
-      </c>
-      <c r="B126" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B127" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B128" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>102</v>
       </c>
-      <c r="B129" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A130" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A131" t="s">
+      <c r="B130" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B131" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A133" s="1" t="s">
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A134" t="s">
+      <c r="B134" t="s">
         <v>105</v>
       </c>
-      <c r="B134" t="s">
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A135" t="s">
+      <c r="B135" t="s">
         <v>107</v>
       </c>
-      <c r="B135" t="s">
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A136" t="s">
+      <c r="B136" t="s">
         <v>109</v>
       </c>
-      <c r="B136" t="s">
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A137" t="s">
+      <c r="B137" t="s">
         <v>111</v>
       </c>
-      <c r="B137" t="s">
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A138" t="s">
-        <v>113</v>
-      </c>
       <c r="B138" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B139" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>113</v>
+      </c>
+      <c r="B140" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>108</v>
+      </c>
+      <c r="B141" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>115</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B142" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A141" t="s">
-        <v>109</v>
-      </c>
-      <c r="B141" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A142" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>112</v>
+      </c>
+      <c r="B143" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>117</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B144" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A143" t="s">
-        <v>113</v>
-      </c>
-      <c r="B143" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A144" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>120</v>
       </c>
-      <c r="B144" t="s">
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A145" t="s">
+      <c r="B147" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A146" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
+      <c r="B150" t="s">
         <v>124</v>
       </c>
-      <c r="B147" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A149" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A150" t="s">
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B151" t="s">
         <v>126</v>
       </c>
-      <c r="B150" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
-        <v>130</v>
-      </c>
-      <c r="B151" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>125</v>
+      </c>
+      <c r="B153" t="s">
         <v>128</v>
       </c>
-      <c r="B153" t="s">
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>129</v>
+      </c>
+      <c r="B154" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A154" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>132</v>
       </c>
-      <c r="B154" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A156" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A157" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A158" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>7</v>
       </c>
       <c r="B161" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1767,7 +1768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrationstest Bildschirm überspringen hinzugefügt
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E95CB1-6BF7-4489-AFFA-7103EF60672A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF2E586-D659-45C0-83FA-6D573532ADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="147">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -449,6 +449,24 @@
   </si>
   <si>
     <t>In der Liste wird die neue KI zusätzlich angezeigt.</t>
+  </si>
+  <si>
+    <t>Test: Bildschirme überspringen</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 "Mensch", für Spieler 2 "KI-Elimination" und klickt auf das Feld "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Die Spielansicht wird angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt abwechselnd selber auf ein freies Feld und löst Züge der KI aus, bis das Spiel beendet ist.</t>
+  </si>
+  <si>
+    <t>Die Checkbox ist nicht mehr mit einem Haken versehen.</t>
+  </si>
+  <si>
+    <t>Die Startansicht wird angezeigt</t>
   </si>
 </sst>
 </file>
@@ -775,15 +793,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B161"/>
+  <dimension ref="A1:B179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.28515625" customWidth="1"/>
+    <col min="1" max="1" width="98.28515625" customWidth="1"/>
     <col min="2" max="2" width="145.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1755,6 +1773,130 @@
       </c>
       <c r="B161" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>142</v>
+      </c>
+      <c r="B164" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>28</v>
+      </c>
+      <c r="B165" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>43</v>
+      </c>
+      <c r="B167" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>10</v>
+      </c>
+      <c r="B168" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>43</v>
+      </c>
+      <c r="B169" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>28</v>
+      </c>
+      <c r="B170" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>29</v>
+      </c>
+      <c r="B171" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>43</v>
+      </c>
+      <c r="B173" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>3</v>
+      </c>
+      <c r="B174" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>29</v>
+      </c>
+      <c r="B175" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>43</v>
+      </c>
+      <c r="B177" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>10</v>
+      </c>
+      <c r="B178" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>43</v>
+      </c>
+      <c r="B179" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kleine Typos in Integrationstests gefixt, Specs für Surface eingetragen
</commit_message>
<xml_diff>
--- a/Integrationstests/Integrationstests.xlsx
+++ b/Integrationstests/Integrationstests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Integrationstests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF2E586-D659-45C0-83FA-6D573532ADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237AAB5C-EFE4-4028-9FBD-B99948A46C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1635" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
   <si>
     <t>Der Nutzer klickt auf das DropDown-Menü für die Auswahl von Spieler 1.</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Der Nutzer klickt auf das "NextMove"-Symbol (="Play"-Symbol mit | rechts).</t>
   </si>
   <si>
-    <t>Das "Play"-Symbol wird durch ein "Pause"-Symbol ersetzt.</t>
-  </si>
-  <si>
     <t>Der Nutzer klickt auf dem Spielfeld auf das Feld rechts oben.</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>Zufällige freie Felder werden von den KIs besetzt.</t>
   </si>
   <si>
-    <t>Der Nutzer klickt auf das "Play"-Symbol, bevor das Spiel beendet ist.</t>
-  </si>
-  <si>
     <t>Keine weiteren Felder werden besetzt.</t>
   </si>
   <si>
@@ -467,6 +461,33 @@
   </si>
   <si>
     <t>Die Startansicht wird angezeigt</t>
+  </si>
+  <si>
+    <t>Leonid Surface</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Windows 11 Pro</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Microsoft Edge Version 120  (64 Bit)</t>
+  </si>
+  <si>
+    <t>Anmerkungen</t>
+  </si>
+  <si>
+    <t>mit Touchdisplay</t>
+  </si>
+  <si>
+    <t>Das "Pause"-Symbol wird durch ein "Play"-Symbol ersetzt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das "Pause"-Symbol, bevor das Spiel beendet ist.</t>
   </si>
 </sst>
 </file>
@@ -795,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A190" sqref="A190"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -836,10 +857,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,15 +868,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +884,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -871,31 +892,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
         <v>59</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -903,23 +924,23 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,57 +948,57 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -985,7 +1006,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -993,7 +1014,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1001,7 +1022,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1009,7 +1030,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,12 +1038,12 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,12 +1051,12 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,31 +1069,31 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1080,15 +1101,15 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1098,12 +1119,12 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1132,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1121,10 +1142,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1153,7 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,15 +1161,15 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1164,43 +1185,43 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" t="s">
         <v>65</v>
-      </c>
-      <c r="B55" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,10 +1231,10 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1223,10 +1244,10 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1234,17 +1255,17 @@
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,17 +1273,17 @@
         <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,32 +1293,32 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1307,191 +1328,191 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B90" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B108" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B114" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>89</v>
+      </c>
+      <c r="B117" t="s">
         <v>90</v>
-      </c>
-      <c r="B117" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,28 +1520,28 @@
         <v>7</v>
       </c>
       <c r="B118" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="B119" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B121" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1530,10 +1551,10 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B123" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1543,31 +1564,31 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" t="s">
         <v>65</v>
-      </c>
-      <c r="B125" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B128" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1577,66 +1598,66 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B130" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B134" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B135" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B136" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B137" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B138" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B139" t="s">
         <v>8</v>
@@ -1644,81 +1665,81 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B141" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B142" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B144" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B147" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B150" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B151" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,43 +1749,43 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B153" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B154" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -1772,41 +1793,41 @@
         <v>7</v>
       </c>
       <c r="B161" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B164" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B165" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B167" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -1814,44 +1835,44 @@
         <v>10</v>
       </c>
       <c r="B168" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B169" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B170" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B171" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B173" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -1859,28 +1880,28 @@
         <v>3</v>
       </c>
       <c r="B174" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B175" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B177" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -1888,15 +1909,15 @@
         <v>10</v>
       </c>
       <c r="B178" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B179" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1906,12 +1927,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651AFE88-806E-4574-AED0-363C8FFDCEFE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>